<commit_message>
feat: Refactor success page and API actions for improved analysis handling
</commit_message>
<xml_diff>
--- a/server/results/keyword_analysis_gsc_all.xlsx
+++ b/server/results/keyword_analysis_gsc_all.xlsx
@@ -473,7 +473,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:N34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -482,12 +482,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="26" customWidth="1" min="1" max="1"/>
+    <col width="50" customWidth="1" min="1" max="1"/>
     <col width="50" customWidth="1" min="2" max="2"/>
     <col width="7" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
     <col width="5" customWidth="1" min="5" max="5"/>
-    <col width="5" customWidth="1" min="6" max="6"/>
+    <col width="4" customWidth="1" min="6" max="6"/>
     <col width="9" customWidth="1" min="7" max="7"/>
     <col width="10" customWidth="1" min="8" max="8"/>
     <col width="8" customWidth="1" min="9" max="9"/>
@@ -573,12 +573,12 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>محرك بحث فيديو</t>
+          <t>dottopia</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>https://scarabio.com/%D8%A3%D9%81%D8%B6%D9%84-%D9%85%D8%AD%D8%B1%D9%83%D8%A7%D8%AA-%D8%A8%D8%AD%D8%AB-%D8%A7%D9%84%D9%81%D9%8A%D8%AF%D9%8A%D9%88/</t>
+          <t>https://dottopia.com/</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr">
@@ -591,9 +591,9 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="E2" s="3" t="inlineStr">
-        <is>
-          <t>NO</t>
+      <c r="E2" s="4" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
       <c r="F2" s="3" t="inlineStr">
@@ -617,62 +617,60 @@
         </is>
       </c>
       <c r="J2" s="2" t="n">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="K2" s="2" t="n">
-        <v>76</v>
-      </c>
-      <c r="L2" s="2" t="inlineStr">
-        <is>
-          <t>31.6%</t>
-        </is>
+        <v>58</v>
+      </c>
+      <c r="L2" s="2" t="n">
+        <v>36.21</v>
       </c>
       <c r="M2" s="2" t="n">
-        <v>1.8</v>
+        <v>1.81</v>
       </c>
       <c r="N2" s="2" t="n">
-        <v>52</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>أفضل محركات بحث الفيديو</t>
+          <t>dotopia</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>https://scarabio.com/%D8%A3%D9%81%D8%B6%D9%84-%D9%85%D8%AD%D8%B1%D9%83%D8%A7%D8%AA-%D8%A8%D8%AD%D8%AB-%D8%A7%D9%84%D9%81%D9%8A%D8%AF%D9%8A%D9%88/</t>
-        </is>
-      </c>
-      <c r="C3" s="4" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="D3" s="4" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="E3" s="4" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="F3" s="4" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="G3" s="4" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="H3" s="4" t="inlineStr">
-        <is>
-          <t>YES</t>
+          <t>https://dottopia.com/</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D3" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E3" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="F3" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G3" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H3" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
       <c r="I3" s="3" t="inlineStr">
@@ -681,32 +679,30 @@
         </is>
       </c>
       <c r="J3" s="2" t="n">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="K3" s="2" t="n">
-        <v>434</v>
-      </c>
-      <c r="L3" s="2" t="inlineStr">
-        <is>
-          <t>4.8%</t>
-        </is>
+        <v>69</v>
+      </c>
+      <c r="L3" s="2" t="n">
+        <v>2.9</v>
       </c>
       <c r="M3" s="2" t="n">
-        <v>4.7</v>
+        <v>4.35</v>
       </c>
       <c r="N3" s="2" t="n">
-        <v>413</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>موقع للبحث عن فيديوهات</t>
+          <t>مؤشرات قياس الأداء التسويقي pdf</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>https://scarabio.com/%D8%A3%D9%81%D8%B6%D9%84-%D9%85%D8%AD%D8%B1%D9%83%D8%A7%D8%AA-%D8%A8%D8%AD%D8%AB-%D8%A7%D9%84%D9%81%D9%8A%D8%AF%D9%8A%D9%88/</t>
+          <t>https://dottopia.com/ar/%D9%85%D8%B9%D8%A7%D9%8A%D9%8A%D8%B1-%D9%82%D9%8A%D8%A7%D8%B3-%D8%A7%D9%84%D8%A3%D8%AF%D8%A7%D8%A1-%D8%A7%D9%84%D8%AA%D8%B3%D9%88%D9%8A%D9%82%D9%8A/</t>
         </is>
       </c>
       <c r="C4" s="3" t="inlineStr">
@@ -745,32 +741,30 @@
         </is>
       </c>
       <c r="J4" s="2" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="K4" s="2" t="n">
-        <v>196</v>
-      </c>
-      <c r="L4" s="2" t="inlineStr">
-        <is>
-          <t>6.6%</t>
-        </is>
+        <v>5</v>
+      </c>
+      <c r="L4" s="2" t="n">
+        <v>40</v>
       </c>
       <c r="M4" s="2" t="n">
-        <v>2.8</v>
+        <v>10.2</v>
       </c>
       <c r="N4" s="2" t="n">
-        <v>183</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>أفضل موقع للبحث بالصور</t>
+          <t>canales digitales de comunicación</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>https://scarabio.com/%D8%A7%D8%AD%D8%B3%D9%86-%D9%85%D8%AD%D8%B1%D9%83-%D8%A8%D8%AD%D8%AB-%D9%84%D9%84%D8%B5%D9%88%D8%B1/</t>
+          <t>https://dottopia.com/types-of-digital-communication-channels/</t>
         </is>
       </c>
       <c r="C5" s="3" t="inlineStr">
@@ -809,32 +803,30 @@
         </is>
       </c>
       <c r="J5" s="2" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="K5" s="2" t="n">
-        <v>69</v>
-      </c>
-      <c r="L5" s="2" t="inlineStr">
-        <is>
-          <t>15.9%</t>
-        </is>
+        <v>14</v>
+      </c>
+      <c r="L5" s="2" t="n">
+        <v>14.29</v>
       </c>
       <c r="M5" s="2" t="n">
-        <v>3.5</v>
+        <v>2.79</v>
       </c>
       <c r="N5" s="2" t="n">
-        <v>58</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>محرك بحث صور</t>
+          <t>digital communication channels</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>https://scarabio.com/%D8%A7%D8%AD%D8%B3%D9%86-%D9%85%D8%AD%D8%B1%D9%83-%D8%A8%D8%AD%D8%AB-%D9%84%D9%84%D8%B5%D9%88%D8%B1/</t>
+          <t>https://dottopia.com/types-of-digital-communication-channels/</t>
         </is>
       </c>
       <c r="C6" s="3" t="inlineStr">
@@ -873,32 +865,30 @@
         </is>
       </c>
       <c r="J6" s="2" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="K6" s="2" t="n">
-        <v>63</v>
-      </c>
-      <c r="L6" s="2" t="inlineStr">
-        <is>
-          <t>17.5%</t>
-        </is>
+        <v>177</v>
+      </c>
+      <c r="L6" s="2" t="n">
+        <v>1.13</v>
       </c>
       <c r="M6" s="2" t="n">
-        <v>4.5</v>
+        <v>3.67</v>
       </c>
       <c r="N6" s="2" t="n">
-        <v>52</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>بحث بالفيديو</t>
+          <t>communication strategies that encourage digital connections</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>https://scarabio.com/%D8%A3%D9%81%D8%B6%D9%84-%D9%85%D8%AD%D8%B1%D9%83%D8%A7%D8%AA-%D8%A8%D8%AD%D8%AB-%D8%A7%D9%84%D9%81%D9%8A%D8%AF%D9%8A%D9%88/</t>
+          <t>https://dottopia.com/what-is-digital-communication-strategy/</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
@@ -937,32 +927,30 @@
         </is>
       </c>
       <c r="J7" s="2" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K7" s="2" t="n">
-        <v>93</v>
-      </c>
-      <c r="L7" s="2" t="inlineStr">
-        <is>
-          <t>6.5%</t>
-        </is>
+        <v>126</v>
+      </c>
+      <c r="L7" s="2" t="n">
+        <v>1.59</v>
       </c>
       <c r="M7" s="2" t="n">
-        <v>9.300000000000001</v>
+        <v>10.91</v>
       </c>
       <c r="N7" s="2" t="n">
-        <v>87</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>موقع البحث عن الصور</t>
+          <t>performance marketing agency</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>https://scarabio.com/%D8%A7%D8%AD%D8%B3%D9%86-%D9%85%D8%AD%D8%B1%D9%83-%D8%A8%D8%AD%D8%AB-%D9%84%D9%84%D8%B5%D9%88%D8%B1/</t>
+          <t>https://dottopia.com/</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
@@ -1001,32 +989,30 @@
         </is>
       </c>
       <c r="J8" s="2" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="K8" s="2" t="n">
-        <v>66</v>
-      </c>
-      <c r="L8" s="2" t="inlineStr">
-        <is>
-          <t>9.1%</t>
-        </is>
+        <v>1</v>
+      </c>
+      <c r="L8" s="2" t="n">
+        <v>100</v>
       </c>
       <c r="M8" s="2" t="n">
-        <v>10.5</v>
+        <v>52</v>
       </c>
       <c r="N8" s="2" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
         <is>
-          <t>أفضل موقع للبحث عن الصور</t>
+          <t>فحص موقعي</t>
         </is>
       </c>
       <c r="B9" s="2" t="inlineStr">
         <is>
-          <t>https://scarabio.com/%D8%A7%D8%AD%D8%B3%D9%86-%D9%85%D8%AD%D8%B1%D9%83-%D8%A8%D8%AD%D8%AB-%D9%84%D9%84%D8%B5%D9%88%D8%B1/</t>
+          <t>https://dottopia.com/ar/%D8%A7%D9%81%D8%B6%D9%84-%D8%A7%D8%AF%D8%A7%D9%87-%D9%84%D9%81%D8%AD%D8%B5-%D8%B3%D9%8A%D9%88-%D9%85%D9%88%D9%82%D8%B9%D9%83/</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
@@ -1065,32 +1051,30 @@
         </is>
       </c>
       <c r="J9" s="2" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K9" s="2" t="n">
-        <v>32</v>
-      </c>
-      <c r="L9" s="2" t="inlineStr">
-        <is>
-          <t>15.6%</t>
-        </is>
+        <v>2</v>
+      </c>
+      <c r="L9" s="2" t="n">
+        <v>50</v>
       </c>
       <c r="M9" s="2" t="n">
-        <v>3.5</v>
+        <v>42</v>
       </c>
       <c r="N9" s="2" t="n">
-        <v>27</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>افضل موقع للبحث عن الصور</t>
+          <t>7 channels of communication</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>https://scarabio.com/%D8%A7%D8%AD%D8%B3%D9%86-%D9%85%D8%AD%D8%B1%D9%83-%D8%A8%D8%AD%D8%AB-%D9%84%D9%84%D8%B5%D9%88%D8%B1/</t>
+          <t>https://dottopia.com/types-of-digital-communication-channels/</t>
         </is>
       </c>
       <c r="C10" s="3" t="inlineStr">
@@ -1129,32 +1113,30 @@
         </is>
       </c>
       <c r="J10" s="2" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K10" s="2" t="n">
-        <v>29</v>
-      </c>
-      <c r="L10" s="2" t="inlineStr">
-        <is>
-          <t>17.2%</t>
-        </is>
+        <v>669</v>
+      </c>
+      <c r="L10" s="2" t="n">
+        <v>0.15</v>
       </c>
       <c r="M10" s="2" t="n">
-        <v>3.9</v>
+        <v>5.65</v>
       </c>
       <c r="N10" s="2" t="n">
-        <v>24</v>
+        <v>668</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>محرك بحث الصور</t>
+          <t>digital communications</t>
         </is>
       </c>
       <c r="B11" s="2" t="inlineStr">
         <is>
-          <t>https://scarabio.com/%D8%A7%D8%AD%D8%B3%D9%86-%D9%85%D8%AD%D8%B1%D9%83-%D8%A8%D8%AD%D8%AB-%D9%84%D9%84%D8%B5%D9%88%D8%B1/</t>
+          <t>https://dottopia.com/types-of-digital-communication-channels/</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr">
@@ -1177,9 +1159,9 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="G11" s="4" t="inlineStr">
-        <is>
-          <t>YES</t>
+      <c r="G11" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
       <c r="H11" s="3" t="inlineStr">
@@ -1193,32 +1175,30 @@
         </is>
       </c>
       <c r="J11" s="2" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K11" s="2" t="n">
-        <v>40</v>
-      </c>
-      <c r="L11" s="2" t="inlineStr">
-        <is>
-          <t>12.5%</t>
-        </is>
+        <v>104</v>
+      </c>
+      <c r="L11" s="2" t="n">
+        <v>0.96</v>
       </c>
       <c r="M11" s="2" t="n">
-        <v>6.3</v>
+        <v>1</v>
       </c>
       <c r="N11" s="2" t="n">
-        <v>35</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>محرك بحث بالصور</t>
+          <t>type of communication channel</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t>https://scarabio.com/%D8%A7%D8%AD%D8%B3%D9%86-%D9%85%D8%AD%D8%B1%D9%83-%D8%A8%D8%AD%D8%AB-%D9%84%D9%84%D8%B5%D9%88%D8%B1/</t>
+          <t>https://dottopia.com/types-of-digital-communication-channels/</t>
         </is>
       </c>
       <c r="C12" s="3" t="inlineStr">
@@ -1257,21 +1237,1383 @@
         </is>
       </c>
       <c r="J12" s="2" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K12" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="L12" s="2" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="M12" s="2" t="n">
+        <v>12.18</v>
+      </c>
+      <c r="N12" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>types of channel in communication</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="inlineStr">
+        <is>
+          <t>https://dottopia.com/types-of-digital-communication-channels/</t>
+        </is>
+      </c>
+      <c r="C13" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D13" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E13" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="F13" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G13" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H13" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I13" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J13" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K13" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="L13" s="2" t="n">
+        <v>1.82</v>
+      </c>
+      <c r="M13" s="2" t="n">
+        <v>5.36</v>
+      </c>
+      <c r="N13" s="2" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>types of digital communication</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="inlineStr">
+        <is>
+          <t>https://dottopia.com/types-of-digital-communication-channels/</t>
+        </is>
+      </c>
+      <c r="C14" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D14" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E14" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="F14" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G14" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H14" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I14" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J14" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K14" s="2" t="n">
+        <v>206</v>
+      </c>
+      <c r="L14" s="2" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="M14" s="2" t="n">
+        <v>7.58</v>
+      </c>
+      <c r="N14" s="2" t="n">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>describe communication strategies that encourage digital connections. include the following: how does each strategy encourage digital connections? does each strategy work all the time? why or why not?</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>https://dottopia.com/what-is-digital-communication-strategy/</t>
+        </is>
+      </c>
+      <c r="C15" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D15" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E15" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="F15" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G15" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H15" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I15" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K15" s="2" t="n">
+        <v>51</v>
+      </c>
+      <c r="L15" s="2" t="n">
+        <v>1.96</v>
+      </c>
+      <c r="M15" s="2" t="n">
+        <v>2.31</v>
+      </c>
+      <c r="N15" s="2" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>digital communication strategy</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="inlineStr">
+        <is>
+          <t>https://dottopia.com/what-is-digital-communication-strategy/</t>
+        </is>
+      </c>
+      <c r="C16" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D16" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E16" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="F16" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G16" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H16" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I16" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J16" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K16" s="2" t="n">
+        <v>476</v>
+      </c>
+      <c r="L16" s="2" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="M16" s="2" t="n">
+        <v>9.289999999999999</v>
+      </c>
+      <c r="N16" s="2" t="n">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>digital marketing communication plan</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="inlineStr">
+        <is>
+          <t>https://dottopia.com/what-is-digital-communication-strategy/</t>
+        </is>
+      </c>
+      <c r="C17" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D17" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E17" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="F17" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G17" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H17" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I17" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J17" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K17" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="L17" s="2" t="n">
+        <v>33.33</v>
+      </c>
+      <c r="M17" s="2" t="n">
+        <v>22.33</v>
+      </c>
+      <c r="N17" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>how does each strategy encourage digital connections?</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="inlineStr">
+        <is>
+          <t>https://dottopia.com/what-is-digital-communication-strategy/</t>
+        </is>
+      </c>
+      <c r="C18" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D18" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E18" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="F18" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G18" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H18" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I18" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J18" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K18" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="L18" s="2" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="M18" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="N18" s="2" t="n">
         <v>29</v>
       </c>
-      <c r="L12" s="2" t="inlineStr">
-        <is>
-          <t>17.2%</t>
-        </is>
-      </c>
-      <c r="M12" s="2" t="n">
-        <v>7.1</v>
-      </c>
-      <c r="N12" s="2" t="n">
-        <v>24</v>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="inlineStr">
+        <is>
+          <t>what is digital communication strategy</t>
+        </is>
+      </c>
+      <c r="B19" s="2" t="inlineStr">
+        <is>
+          <t>https://dottopia.com/what-is-digital-communication-strategy/</t>
+        </is>
+      </c>
+      <c r="C19" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D19" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E19" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="F19" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G19" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H19" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I19" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J19" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K19" s="2" t="n">
+        <v>94</v>
+      </c>
+      <c r="L19" s="2" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="M19" s="2" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="N19" s="2" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>advertising agencies</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="inlineStr">
+        <is>
+          <t>https://dottopia.com/</t>
+        </is>
+      </c>
+      <c r="C20" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D20" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E20" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="F20" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G20" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H20" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I20" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M20" s="2" t="n">
+        <v>93</v>
+      </c>
+      <c r="N20" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="inlineStr">
+        <is>
+          <t>advertising agency cairo</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="inlineStr">
+        <is>
+          <t>https://dottopia.com/</t>
+        </is>
+      </c>
+      <c r="C21" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D21" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E21" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="F21" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G21" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H21" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I21" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M21" s="2" t="n">
+        <v>88</v>
+      </c>
+      <c r="N21" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>advertising agency egypt</t>
+        </is>
+      </c>
+      <c r="B22" s="2" t="inlineStr">
+        <is>
+          <t>https://dottopia.com/</t>
+        </is>
+      </c>
+      <c r="C22" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D22" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E22" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="F22" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G22" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H22" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I22" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M22" s="2" t="n">
+        <v>95</v>
+      </c>
+      <c r="N22" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="inlineStr">
+        <is>
+          <t>arabic digital marketing agency</t>
+        </is>
+      </c>
+      <c r="B23" s="2" t="inlineStr">
+        <is>
+          <t>https://dottopia.com/</t>
+        </is>
+      </c>
+      <c r="C23" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D23" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E23" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="F23" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G23" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H23" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I23" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M23" s="2" t="n">
+        <v>99</v>
+      </c>
+      <c r="N23" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="inlineStr">
+        <is>
+          <t>arma group egypt</t>
+        </is>
+      </c>
+      <c r="B24" s="2" t="inlineStr">
+        <is>
+          <t>https://dottopia.com/</t>
+        </is>
+      </c>
+      <c r="C24" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D24" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E24" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="F24" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G24" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H24" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I24" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K24" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M24" s="2" t="n">
+        <v>44</v>
+      </c>
+      <c r="N24" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="inlineStr">
+        <is>
+          <t>best digital marketing agencies in egypt</t>
+        </is>
+      </c>
+      <c r="B25" s="2" t="inlineStr">
+        <is>
+          <t>https://dottopia.com/</t>
+        </is>
+      </c>
+      <c r="C25" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D25" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E25" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="F25" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G25" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H25" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I25" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K25" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M25" s="2" t="n">
+        <v>89</v>
+      </c>
+      <c r="N25" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="inlineStr">
+        <is>
+          <t>best digital marketing agency egypt</t>
+        </is>
+      </c>
+      <c r="B26" s="2" t="inlineStr">
+        <is>
+          <t>https://dottopia.com/</t>
+        </is>
+      </c>
+      <c r="C26" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D26" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E26" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="F26" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G26" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H26" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I26" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K26" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M26" s="2" t="n">
+        <v>93</v>
+      </c>
+      <c r="N26" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="inlineStr">
+        <is>
+          <t>companies marketing</t>
+        </is>
+      </c>
+      <c r="B27" s="2" t="inlineStr">
+        <is>
+          <t>https://dottopia.com/</t>
+        </is>
+      </c>
+      <c r="C27" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D27" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E27" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="F27" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G27" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H27" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I27" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M27" s="2" t="n">
+        <v>105</v>
+      </c>
+      <c r="N27" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="inlineStr">
+        <is>
+          <t>digital advertising</t>
+        </is>
+      </c>
+      <c r="B28" s="2" t="inlineStr">
+        <is>
+          <t>https://dottopia.com/</t>
+        </is>
+      </c>
+      <c r="C28" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D28" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E28" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="F28" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G28" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H28" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I28" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K28" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M28" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="N28" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="inlineStr">
+        <is>
+          <t>digital agency egypt</t>
+        </is>
+      </c>
+      <c r="B29" s="2" t="inlineStr">
+        <is>
+          <t>https://dottopia.com/</t>
+        </is>
+      </c>
+      <c r="C29" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D29" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E29" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="F29" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G29" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H29" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I29" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K29" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M29" s="2" t="n">
+        <v>96</v>
+      </c>
+      <c r="N29" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="inlineStr">
+        <is>
+          <t>digital marketing agency italy food</t>
+        </is>
+      </c>
+      <c r="B30" s="2" t="inlineStr">
+        <is>
+          <t>https://dottopia.com/</t>
+        </is>
+      </c>
+      <c r="C30" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D30" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E30" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="F30" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G30" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H30" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I30" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K30" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="L30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M30" s="2" t="n">
+        <v>82.75</v>
+      </c>
+      <c r="N30" s="2" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="inlineStr">
+        <is>
+          <t>dot advertising agency</t>
+        </is>
+      </c>
+      <c r="B31" s="2" t="inlineStr">
+        <is>
+          <t>https://dottopia.com/</t>
+        </is>
+      </c>
+      <c r="C31" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D31" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E31" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="F31" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G31" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H31" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I31" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K31" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M31" s="2" t="n">
+        <v>42</v>
+      </c>
+      <c r="N31" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="inlineStr">
+        <is>
+          <t>fintech advertising agency</t>
+        </is>
+      </c>
+      <c r="B32" s="2" t="inlineStr">
+        <is>
+          <t>https://dottopia.com/</t>
+        </is>
+      </c>
+      <c r="C32" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D32" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E32" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="F32" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G32" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H32" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I32" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K32" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="L32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M32" s="2" t="n">
+        <v>10.69</v>
+      </c>
+      <c r="N32" s="2" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="inlineStr">
+        <is>
+          <t>influencers marketing agency toys italy</t>
+        </is>
+      </c>
+      <c r="B33" s="2" t="inlineStr">
+        <is>
+          <t>https://dottopia.com/</t>
+        </is>
+      </c>
+      <c r="C33" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D33" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E33" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="F33" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G33" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H33" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I33" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J33" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K33" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="L33" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M33" s="2" t="n">
+        <v>79</v>
+      </c>
+      <c r="N33" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="inlineStr">
+        <is>
+          <t>leadin top</t>
+        </is>
+      </c>
+      <c r="B34" s="2" t="inlineStr">
+        <is>
+          <t>https://dottopia.com/</t>
+        </is>
+      </c>
+      <c r="C34" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D34" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E34" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="F34" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G34" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H34" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I34" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K34" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="L34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M34" s="2" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="N34" s="2" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1285,7 +2627,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1295,7 +2637,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="60" customWidth="1" min="1" max="1"/>
-    <col width="24" customWidth="1" min="2" max="2"/>
+    <col width="30" customWidth="1" min="2" max="2"/>
     <col width="80" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
@@ -1319,34 +2661,85 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>https://scarabio.com/%D8%A3%D9%81%D8%B6%D9%84-%D9%85%D8%AD%D8%B1%D9%83%D8%A7%D8%AA-%D8%A8%D8%AD%D8%AB-%D8%A7%D9%84%D9%81%D9%8A%D8%AF%D9%8A%D9%88/</t>
+          <t>https://dottopia.com/</t>
         </is>
       </c>
       <c r="B2" s="5" t="inlineStr">
         <is>
-          <t>محرك بحث فيديو</t>
+          <t>dottopia</t>
         </is>
       </c>
       <c r="C2" s="6" t="inlineStr">
         <is>
-          <t>أفضل محركات بحث الفيديو; موقع للبحث عن فيديوهات; بحث بالفيديو</t>
+          <t>dotopia; performance marketing agency; advertising agencies; advertising agency cairo; advertising agency egypt; arabic digital marketing agency</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>https://scarabio.com/%D8%A7%D8%AD%D8%B3%D9%86-%D9%85%D8%AD%D8%B1%D9%83-%D8%A8%D8%AD%D8%AB-%D9%84%D9%84%D8%B5%D9%88%D8%B1/</t>
+          <t>https://dottopia.com/ar/%D8%A7%D9%81%D8%B6%D9%84-%D8%A7%D8%AF%D8%A7%D9%87-%D9%84%D9%81%D8%AD%D8%B5-%D8%B3%D9%8A%D9%88-%D9%85%D9%88%D9%82%D8%B9%D9%83/</t>
         </is>
       </c>
       <c r="B3" s="5" t="inlineStr">
         <is>
-          <t>أفضل موقع للبحث بالصور</t>
+          <t>فحص موقعي</t>
         </is>
       </c>
       <c r="C3" s="6" t="inlineStr">
         <is>
-          <t>محرك بحث صور; موقع البحث عن الصور; أفضل موقع للبحث عن الصور; افضل موقع للبحث عن الصور; محرك بحث الصور; محرك بحث بالصور</t>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>https://dottopia.com/ar/%D9%85%D8%B9%D8%A7%D9%8A%D9%8A%D8%B1-%D9%82%D9%8A%D8%A7%D8%B3-%D8%A7%D9%84%D8%A3%D8%AF%D8%A7%D8%A1-%D8%A7%D9%84%D8%AA%D8%B3%D9%88%D9%8A%D9%82%D9%8A/</t>
+        </is>
+      </c>
+      <c r="B4" s="5" t="inlineStr">
+        <is>
+          <t>مؤشرات قياس الأداء التسويقي pdf</t>
+        </is>
+      </c>
+      <c r="C4" s="6" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>https://dottopia.com/types-of-digital-communication-channels/</t>
+        </is>
+      </c>
+      <c r="B5" s="5" t="inlineStr">
+        <is>
+          <t>canales digitales de comunicación</t>
+        </is>
+      </c>
+      <c r="C5" s="6" t="inlineStr">
+        <is>
+          <t>digital communication channels; 7 channels of communication; digital communications; type of communication channel; types of channel in communication; types of digital communication</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>https://dottopia.com/what-is-digital-communication-strategy/</t>
+        </is>
+      </c>
+      <c r="B6" s="5" t="inlineStr">
+        <is>
+          <t>communication strategies that encourage digital connections</t>
+        </is>
+      </c>
+      <c r="C6" s="6" t="inlineStr">
+        <is>
+          <t>describe communication strategies that encourage digital connections. include the following: how does each strategy encourage digital connections? does each strategy work all the time? why or why not?; digital communication strategy; digital marketing communication plan; how does each strategy encourage digital connections?; what is digital communication strategy</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: enhance logging for Google Analysis and OAuth processes
</commit_message>
<xml_diff>
--- a/server/results/keyword_analysis_gsc_all.xlsx
+++ b/server/results/keyword_analysis_gsc_all.xlsx
@@ -473,7 +473,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N34"/>
+  <dimension ref="A1:N52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -483,7 +483,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="50" customWidth="1" min="1" max="1"/>
-    <col width="50" customWidth="1" min="2" max="2"/>
+    <col width="33" customWidth="1" min="2" max="2"/>
     <col width="7" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
     <col width="5" customWidth="1" min="5" max="5"/>
@@ -573,12 +573,12 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>dottopia</t>
+          <t>goocast</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>https://dottopia.com/</t>
+          <t>https://goocast.net/</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr">
@@ -617,30 +617,30 @@
         </is>
       </c>
       <c r="J2" s="2" t="n">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="K2" s="2" t="n">
-        <v>58</v>
+        <v>183</v>
       </c>
       <c r="L2" s="2" t="n">
-        <v>36.21</v>
+        <v>34.43</v>
       </c>
       <c r="M2" s="2" t="n">
-        <v>1.81</v>
+        <v>1.04</v>
       </c>
       <c r="N2" s="2" t="n">
-        <v>37</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>dotopia</t>
+          <t>podcast studio cairo</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>https://dottopia.com/</t>
+          <t>https://goocast.net/</t>
         </is>
       </c>
       <c r="C3" s="3" t="inlineStr">
@@ -679,30 +679,30 @@
         </is>
       </c>
       <c r="J3" s="2" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="K3" s="2" t="n">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="L3" s="2" t="n">
-        <v>2.9</v>
+        <v>6.82</v>
       </c>
       <c r="M3" s="2" t="n">
-        <v>4.35</v>
+        <v>5.3</v>
       </c>
       <c r="N3" s="2" t="n">
-        <v>67</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>مؤشرات قياس الأداء التسويقي pdf</t>
+          <t>podcast studio</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>https://dottopia.com/ar/%D9%85%D8%B9%D8%A7%D9%8A%D9%8A%D8%B1-%D9%82%D9%8A%D8%A7%D8%B3-%D8%A7%D9%84%D8%A3%D8%AF%D8%A7%D8%A1-%D8%A7%D9%84%D8%AA%D8%B3%D9%88%D9%8A%D9%82%D9%8A/</t>
+          <t>https://goocast.net/</t>
         </is>
       </c>
       <c r="C4" s="3" t="inlineStr">
@@ -744,27 +744,27 @@
         <v>2</v>
       </c>
       <c r="K4" s="2" t="n">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="L4" s="2" t="n">
-        <v>40</v>
+        <v>3.39</v>
       </c>
       <c r="M4" s="2" t="n">
-        <v>10.2</v>
+        <v>9.1</v>
       </c>
       <c r="N4" s="2" t="n">
-        <v>3</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>canales digitales de comunicación</t>
+          <t>podcast studios</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>https://dottopia.com/types-of-digital-communication-channels/</t>
+          <t>https://goocast.net/</t>
         </is>
       </c>
       <c r="C5" s="3" t="inlineStr">
@@ -806,27 +806,27 @@
         <v>2</v>
       </c>
       <c r="K5" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="L5" s="2" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="M5" s="2" t="n">
+        <v>5.69</v>
+      </c>
+      <c r="N5" s="2" t="n">
         <v>14</v>
-      </c>
-      <c r="L5" s="2" t="n">
-        <v>14.29</v>
-      </c>
-      <c r="M5" s="2" t="n">
-        <v>2.79</v>
-      </c>
-      <c r="N5" s="2" t="n">
-        <v>12</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>digital communication channels</t>
+          <t>book podcast studio</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>https://dottopia.com/types-of-digital-communication-channels/</t>
+          <t>https://goocast.net/</t>
         </is>
       </c>
       <c r="C6" s="3" t="inlineStr">
@@ -865,30 +865,30 @@
         </is>
       </c>
       <c r="J6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="M6" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="K6" s="2" t="n">
-        <v>177</v>
-      </c>
-      <c r="L6" s="2" t="n">
-        <v>1.13</v>
-      </c>
-      <c r="M6" s="2" t="n">
-        <v>3.67</v>
-      </c>
       <c r="N6" s="2" t="n">
-        <v>175</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>communication strategies that encourage digital connections</t>
+          <t>podcast locations near me</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>https://dottopia.com/what-is-digital-communication-strategy/</t>
+          <t>https://goocast.net/</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
@@ -927,30 +927,30 @@
         </is>
       </c>
       <c r="J7" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K7" s="2" t="n">
-        <v>126</v>
+        <v>1</v>
       </c>
       <c r="L7" s="2" t="n">
-        <v>1.59</v>
+        <v>100</v>
       </c>
       <c r="M7" s="2" t="n">
-        <v>10.91</v>
+        <v>1</v>
       </c>
       <c r="N7" s="2" t="n">
-        <v>124</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>performance marketing agency</t>
+          <t>podcast production studio</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>https://dottopia.com/</t>
+          <t>https://goocast.net/</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
@@ -992,27 +992,27 @@
         <v>1</v>
       </c>
       <c r="K8" s="2" t="n">
-        <v>1</v>
+        <v>205</v>
       </c>
       <c r="L8" s="2" t="n">
-        <v>100</v>
+        <v>0.49</v>
       </c>
       <c r="M8" s="2" t="n">
-        <v>52</v>
+        <v>48.56</v>
       </c>
       <c r="N8" s="2" t="n">
-        <v>0</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
         <is>
-          <t>فحص موقعي</t>
+          <t>audio production agency</t>
         </is>
       </c>
       <c r="B9" s="2" t="inlineStr">
         <is>
-          <t>https://dottopia.com/ar/%D8%A7%D9%81%D8%B6%D9%84-%D8%A7%D8%AF%D8%A7%D9%87-%D9%84%D9%81%D8%AD%D8%B5-%D8%B3%D9%8A%D9%88-%D9%85%D9%88%D9%82%D8%B9%D9%83/</t>
+          <t>https://goocast.net/</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
@@ -1051,16 +1051,16 @@
         </is>
       </c>
       <c r="J9" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K9" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L9" s="2" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="M9" s="2" t="n">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="N9" s="2" t="n">
         <v>1</v>
@@ -1069,12 +1069,12 @@
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>7 channels of communication</t>
+          <t>best podcast studio</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>https://dottopia.com/types-of-digital-communication-channels/</t>
+          <t>https://goocast.net/</t>
         </is>
       </c>
       <c r="C10" s="3" t="inlineStr">
@@ -1113,30 +1113,30 @@
         </is>
       </c>
       <c r="J10" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K10" s="2" t="n">
-        <v>669</v>
+        <v>1</v>
       </c>
       <c r="L10" s="2" t="n">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="M10" s="2" t="n">
-        <v>5.65</v>
+        <v>89</v>
       </c>
       <c r="N10" s="2" t="n">
-        <v>668</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>digital communications</t>
+          <t>corporate podcast production</t>
         </is>
       </c>
       <c r="B11" s="2" t="inlineStr">
         <is>
-          <t>https://dottopia.com/types-of-digital-communication-channels/</t>
+          <t>https://goocast.net/</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr">
@@ -1175,30 +1175,30 @@
         </is>
       </c>
       <c r="J11" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K11" s="2" t="n">
-        <v>104</v>
+        <v>1</v>
       </c>
       <c r="L11" s="2" t="n">
-        <v>0.96</v>
+        <v>0</v>
       </c>
       <c r="M11" s="2" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="N11" s="2" t="n">
-        <v>103</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>type of communication channel</t>
+          <t>goo cast</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t>https://dottopia.com/types-of-digital-communication-channels/</t>
+          <t>https://goocast.net/</t>
         </is>
       </c>
       <c r="C12" s="3" t="inlineStr">
@@ -1237,30 +1237,30 @@
         </is>
       </c>
       <c r="J12" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K12" s="2" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="L12" s="2" t="n">
-        <v>9.09</v>
+        <v>0</v>
       </c>
       <c r="M12" s="2" t="n">
-        <v>12.18</v>
+        <v>5.57</v>
       </c>
       <c r="N12" s="2" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>types of channel in communication</t>
+          <t>ikea podcast studio</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
         <is>
-          <t>https://dottopia.com/types-of-digital-communication-channels/</t>
+          <t>https://goocast.net/</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr">
@@ -1299,30 +1299,30 @@
         </is>
       </c>
       <c r="J13" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K13" s="2" t="n">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="L13" s="2" t="n">
-        <v>1.82</v>
+        <v>0</v>
       </c>
       <c r="M13" s="2" t="n">
-        <v>5.36</v>
+        <v>5.2</v>
       </c>
       <c r="N13" s="2" t="n">
-        <v>54</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>types of digital communication</t>
+          <t>maxcast studio</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
-          <t>https://dottopia.com/types-of-digital-communication-channels/</t>
+          <t>https://goocast.net/</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr">
@@ -1361,30 +1361,30 @@
         </is>
       </c>
       <c r="J14" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K14" s="2" t="n">
-        <v>206</v>
+        <v>1</v>
       </c>
       <c r="L14" s="2" t="n">
-        <v>0.49</v>
+        <v>0</v>
       </c>
       <c r="M14" s="2" t="n">
-        <v>7.58</v>
+        <v>23</v>
       </c>
       <c r="N14" s="2" t="n">
-        <v>205</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>describe communication strategies that encourage digital connections. include the following: how does each strategy encourage digital connections? does each strategy work all the time? why or why not?</t>
+          <t>media production agency in egypt</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
         <is>
-          <t>https://dottopia.com/what-is-digital-communication-strategy/</t>
+          <t>https://goocast.net/</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
@@ -1423,30 +1423,30 @@
         </is>
       </c>
       <c r="J15" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K15" s="2" t="n">
-        <v>51</v>
+        <v>10</v>
       </c>
       <c r="L15" s="2" t="n">
-        <v>1.96</v>
+        <v>0</v>
       </c>
       <c r="M15" s="2" t="n">
-        <v>2.31</v>
+        <v>68</v>
       </c>
       <c r="N15" s="2" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t>digital communication strategy</t>
+          <t>media production egypt</t>
         </is>
       </c>
       <c r="B16" s="2" t="inlineStr">
         <is>
-          <t>https://dottopia.com/what-is-digital-communication-strategy/</t>
+          <t>https://goocast.net/</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr">
@@ -1485,30 +1485,30 @@
         </is>
       </c>
       <c r="J16" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K16" s="2" t="n">
-        <v>476</v>
+        <v>1</v>
       </c>
       <c r="L16" s="2" t="n">
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="M16" s="2" t="n">
-        <v>9.289999999999999</v>
+        <v>114</v>
       </c>
       <c r="N16" s="2" t="n">
-        <v>475</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>digital marketing communication plan</t>
+          <t>media production studio</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
         <is>
-          <t>https://dottopia.com/what-is-digital-communication-strategy/</t>
+          <t>https://goocast.net/</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
@@ -1547,30 +1547,30 @@
         </is>
       </c>
       <c r="J17" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K17" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L17" s="2" t="n">
-        <v>33.33</v>
+        <v>0</v>
       </c>
       <c r="M17" s="2" t="n">
-        <v>22.33</v>
+        <v>10</v>
       </c>
       <c r="N17" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="inlineStr">
         <is>
-          <t>how does each strategy encourage digital connections?</t>
+          <t>music studio</t>
         </is>
       </c>
       <c r="B18" s="2" t="inlineStr">
         <is>
-          <t>https://dottopia.com/what-is-digital-communication-strategy/</t>
+          <t>https://goocast.net/</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
@@ -1609,30 +1609,30 @@
         </is>
       </c>
       <c r="J18" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K18" s="2" t="n">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="L18" s="2" t="n">
-        <v>3.33</v>
+        <v>0</v>
       </c>
       <c r="M18" s="2" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="N18" s="2" t="n">
-        <v>29</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="inlineStr">
         <is>
-          <t>what is digital communication strategy</t>
+          <t>music studio near me</t>
         </is>
       </c>
       <c r="B19" s="2" t="inlineStr">
         <is>
-          <t>https://dottopia.com/what-is-digital-communication-strategy/</t>
+          <t>https://goocast.net/</t>
         </is>
       </c>
       <c r="C19" s="3" t="inlineStr">
@@ -1671,30 +1671,30 @@
         </is>
       </c>
       <c r="J19" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K19" s="2" t="n">
-        <v>94</v>
+        <v>1</v>
       </c>
       <c r="L19" s="2" t="n">
-        <v>1.06</v>
+        <v>0</v>
       </c>
       <c r="M19" s="2" t="n">
-        <v>1.4</v>
+        <v>93</v>
       </c>
       <c r="N19" s="2" t="n">
-        <v>93</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="inlineStr">
         <is>
-          <t>advertising agencies</t>
+          <t>phocast studios, broadcasting &amp; media production company, toledo</t>
         </is>
       </c>
       <c r="B20" s="2" t="inlineStr">
         <is>
-          <t>https://dottopia.com/</t>
+          <t>https://goocast.net/</t>
         </is>
       </c>
       <c r="C20" s="3" t="inlineStr">
@@ -1736,27 +1736,27 @@
         <v>0</v>
       </c>
       <c r="K20" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L20" s="2" t="n">
         <v>0</v>
       </c>
       <c r="M20" s="2" t="n">
-        <v>93</v>
+        <v>19.5</v>
       </c>
       <c r="N20" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>advertising agency cairo</t>
+          <t>pod cast studio</t>
         </is>
       </c>
       <c r="B21" s="2" t="inlineStr">
         <is>
-          <t>https://dottopia.com/</t>
+          <t>https://goocast.net/</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr">
@@ -1798,27 +1798,27 @@
         <v>0</v>
       </c>
       <c r="K21" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L21" s="2" t="n">
         <v>0</v>
       </c>
       <c r="M21" s="2" t="n">
-        <v>88</v>
+        <v>7.5</v>
       </c>
       <c r="N21" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>advertising agency egypt</t>
+          <t>podcast camera equipment</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
         <is>
-          <t>https://dottopia.com/</t>
+          <t>https://goocast.net/</t>
         </is>
       </c>
       <c r="C22" s="3" t="inlineStr">
@@ -1866,7 +1866,7 @@
         <v>0</v>
       </c>
       <c r="M22" s="2" t="n">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="N22" s="2" t="n">
         <v>1</v>
@@ -1875,12 +1875,12 @@
     <row r="23">
       <c r="A23" s="2" t="inlineStr">
         <is>
-          <t>arabic digital marketing agency</t>
+          <t>podcast egypt</t>
         </is>
       </c>
       <c r="B23" s="2" t="inlineStr">
         <is>
-          <t>https://dottopia.com/</t>
+          <t>https://goocast.net/</t>
         </is>
       </c>
       <c r="C23" s="3" t="inlineStr">
@@ -1928,7 +1928,7 @@
         <v>0</v>
       </c>
       <c r="M23" s="2" t="n">
-        <v>99</v>
+        <v>55</v>
       </c>
       <c r="N23" s="2" t="n">
         <v>1</v>
@@ -1937,12 +1937,12 @@
     <row r="24">
       <c r="A24" s="2" t="inlineStr">
         <is>
-          <t>arma group egypt</t>
+          <t>podcast production</t>
         </is>
       </c>
       <c r="B24" s="2" t="inlineStr">
         <is>
-          <t>https://dottopia.com/</t>
+          <t>https://goocast.net/</t>
         </is>
       </c>
       <c r="C24" s="3" t="inlineStr">
@@ -1984,27 +1984,27 @@
         <v>0</v>
       </c>
       <c r="K24" s="2" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="L24" s="2" t="n">
         <v>0</v>
       </c>
       <c r="M24" s="2" t="n">
-        <v>44</v>
+        <v>11.3</v>
       </c>
       <c r="N24" s="2" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="inlineStr">
         <is>
-          <t>best digital marketing agencies in egypt</t>
+          <t>podcast production companies</t>
         </is>
       </c>
       <c r="B25" s="2" t="inlineStr">
         <is>
-          <t>https://dottopia.com/</t>
+          <t>https://goocast.net/</t>
         </is>
       </c>
       <c r="C25" s="3" t="inlineStr">
@@ -2046,27 +2046,27 @@
         <v>0</v>
       </c>
       <c r="K25" s="2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L25" s="2" t="n">
         <v>0</v>
       </c>
       <c r="M25" s="2" t="n">
-        <v>89</v>
+        <v>5.75</v>
       </c>
       <c r="N25" s="2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="inlineStr">
         <is>
-          <t>best digital marketing agency egypt</t>
+          <t>podcast production studios</t>
         </is>
       </c>
       <c r="B26" s="2" t="inlineStr">
         <is>
-          <t>https://dottopia.com/</t>
+          <t>https://goocast.net/</t>
         </is>
       </c>
       <c r="C26" s="3" t="inlineStr">
@@ -2114,7 +2114,7 @@
         <v>0</v>
       </c>
       <c r="M26" s="2" t="n">
-        <v>93</v>
+        <v>6</v>
       </c>
       <c r="N26" s="2" t="n">
         <v>1</v>
@@ -2123,12 +2123,12 @@
     <row r="27">
       <c r="A27" s="2" t="inlineStr">
         <is>
-          <t>companies marketing</t>
+          <t>podcast recording studio</t>
         </is>
       </c>
       <c r="B27" s="2" t="inlineStr">
         <is>
-          <t>https://dottopia.com/</t>
+          <t>https://goocast.net/</t>
         </is>
       </c>
       <c r="C27" s="3" t="inlineStr">
@@ -2176,7 +2176,7 @@
         <v>0</v>
       </c>
       <c r="M27" s="2" t="n">
-        <v>105</v>
+        <v>5</v>
       </c>
       <c r="N27" s="2" t="n">
         <v>1</v>
@@ -2185,12 +2185,12 @@
     <row r="28">
       <c r="A28" s="2" t="inlineStr">
         <is>
-          <t>digital advertising</t>
+          <t>podcast shooting agency</t>
         </is>
       </c>
       <c r="B28" s="2" t="inlineStr">
         <is>
-          <t>https://dottopia.com/</t>
+          <t>https://goocast.net/</t>
         </is>
       </c>
       <c r="C28" s="3" t="inlineStr">
@@ -2232,27 +2232,27 @@
         <v>0</v>
       </c>
       <c r="K28" s="2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L28" s="2" t="n">
         <v>0</v>
       </c>
       <c r="M28" s="2" t="n">
-        <v>4</v>
+        <v>44.67</v>
       </c>
       <c r="N28" s="2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="inlineStr">
         <is>
-          <t>digital agency egypt</t>
+          <t>podcast shooting service</t>
         </is>
       </c>
       <c r="B29" s="2" t="inlineStr">
         <is>
-          <t>https://dottopia.com/</t>
+          <t>https://goocast.net/</t>
         </is>
       </c>
       <c r="C29" s="3" t="inlineStr">
@@ -2294,27 +2294,27 @@
         <v>0</v>
       </c>
       <c r="K29" s="2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L29" s="2" t="n">
         <v>0</v>
       </c>
       <c r="M29" s="2" t="n">
-        <v>96</v>
+        <v>80.75</v>
       </c>
       <c r="N29" s="2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="inlineStr">
         <is>
-          <t>digital marketing agency italy food</t>
+          <t>podcast shooting studio near me</t>
         </is>
       </c>
       <c r="B30" s="2" t="inlineStr">
         <is>
-          <t>https://dottopia.com/</t>
+          <t>https://goocast.net/</t>
         </is>
       </c>
       <c r="C30" s="3" t="inlineStr">
@@ -2356,27 +2356,27 @@
         <v>0</v>
       </c>
       <c r="K30" s="2" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="L30" s="2" t="n">
         <v>0</v>
       </c>
       <c r="M30" s="2" t="n">
-        <v>82.75</v>
+        <v>7</v>
       </c>
       <c r="N30" s="2" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="inlineStr">
         <is>
-          <t>dot advertising agency</t>
+          <t>podcast studio for rent</t>
         </is>
       </c>
       <c r="B31" s="2" t="inlineStr">
         <is>
-          <t>https://dottopia.com/</t>
+          <t>https://goocast.net/</t>
         </is>
       </c>
       <c r="C31" s="3" t="inlineStr">
@@ -2424,7 +2424,7 @@
         <v>0</v>
       </c>
       <c r="M31" s="2" t="n">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="N31" s="2" t="n">
         <v>1</v>
@@ -2433,12 +2433,12 @@
     <row r="32">
       <c r="A32" s="2" t="inlineStr">
         <is>
-          <t>fintech advertising agency</t>
+          <t>podcast studio near me</t>
         </is>
       </c>
       <c r="B32" s="2" t="inlineStr">
         <is>
-          <t>https://dottopia.com/</t>
+          <t>https://goocast.net/</t>
         </is>
       </c>
       <c r="C32" s="3" t="inlineStr">
@@ -2480,27 +2480,27 @@
         <v>0</v>
       </c>
       <c r="K32" s="2" t="n">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="L32" s="2" t="n">
         <v>0</v>
       </c>
       <c r="M32" s="2" t="n">
-        <v>10.69</v>
+        <v>16.5</v>
       </c>
       <c r="N32" s="2" t="n">
-        <v>16</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="inlineStr">
         <is>
-          <t>influencers marketing agency toys italy</t>
+          <t>podcasts studio</t>
         </is>
       </c>
       <c r="B33" s="2" t="inlineStr">
         <is>
-          <t>https://dottopia.com/</t>
+          <t>https://goocast.net/</t>
         </is>
       </c>
       <c r="C33" s="3" t="inlineStr">
@@ -2542,27 +2542,27 @@
         <v>0</v>
       </c>
       <c r="K33" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L33" s="2" t="n">
         <v>0</v>
       </c>
       <c r="M33" s="2" t="n">
-        <v>79</v>
+        <v>1.5</v>
       </c>
       <c r="N33" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="inlineStr">
         <is>
-          <t>leadin top</t>
+          <t>podcasts studios</t>
         </is>
       </c>
       <c r="B34" s="2" t="inlineStr">
         <is>
-          <t>https://dottopia.com/</t>
+          <t>https://goocast.net/</t>
         </is>
       </c>
       <c r="C34" s="3" t="inlineStr">
@@ -2604,16 +2604,1132 @@
         <v>0</v>
       </c>
       <c r="K34" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M34" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="N34" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="inlineStr">
+        <is>
+          <t>rent podcast studio</t>
+        </is>
+      </c>
+      <c r="B35" s="2" t="inlineStr">
+        <is>
+          <t>https://goocast.net/</t>
+        </is>
+      </c>
+      <c r="C35" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D35" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E35" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="F35" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G35" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H35" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I35" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K35" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M35" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="N35" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="inlineStr">
+        <is>
+          <t>rent podcast studio near me</t>
+        </is>
+      </c>
+      <c r="B36" s="2" t="inlineStr">
+        <is>
+          <t>https://goocast.net/</t>
+        </is>
+      </c>
+      <c r="C36" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D36" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E36" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="F36" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G36" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H36" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I36" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K36" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M36" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="N36" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="inlineStr">
+        <is>
+          <t>seo in egypt podcast</t>
+        </is>
+      </c>
+      <c r="B37" s="2" t="inlineStr">
+        <is>
+          <t>https://goocast.net/</t>
+        </is>
+      </c>
+      <c r="C37" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D37" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E37" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="F37" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G37" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H37" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I37" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J37" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K37" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="L37" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M37" s="2" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="N37" s="2" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="inlineStr">
+        <is>
+          <t>studio for podcast</t>
+        </is>
+      </c>
+      <c r="B38" s="2" t="inlineStr">
+        <is>
+          <t>https://goocast.net/</t>
+        </is>
+      </c>
+      <c r="C38" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D38" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E38" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="F38" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G38" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H38" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I38" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J38" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K38" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="L34" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M34" s="2" t="n">
-        <v>8.5</v>
-      </c>
-      <c r="N34" s="2" t="n">
+      <c r="L38" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M38" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="N38" s="2" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="2" t="inlineStr">
+        <is>
+          <t>studio podcast</t>
+        </is>
+      </c>
+      <c r="B39" s="2" t="inlineStr">
+        <is>
+          <t>https://goocast.net/</t>
+        </is>
+      </c>
+      <c r="C39" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D39" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E39" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="F39" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G39" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H39" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I39" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K39" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="L39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M39" s="2" t="n">
+        <v>7.33</v>
+      </c>
+      <c r="N39" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="inlineStr">
+        <is>
+          <t>studios for podcast</t>
+        </is>
+      </c>
+      <c r="B40" s="2" t="inlineStr">
+        <is>
+          <t>https://goocast.net/</t>
+        </is>
+      </c>
+      <c r="C40" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D40" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E40" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="F40" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G40" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H40" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I40" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K40" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M40" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="N40" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="2" t="inlineStr">
+        <is>
+          <t>the podcast production</t>
+        </is>
+      </c>
+      <c r="B41" s="2" t="inlineStr">
+        <is>
+          <t>https://goocast.net/</t>
+        </is>
+      </c>
+      <c r="C41" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D41" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E41" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="F41" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G41" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H41" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I41" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K41" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="L41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M41" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="N41" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="inlineStr">
+        <is>
+          <t>the podcast productions</t>
+        </is>
+      </c>
+      <c r="B42" s="2" t="inlineStr">
+        <is>
+          <t>https://goocast.net/</t>
+        </is>
+      </c>
+      <c r="C42" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D42" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E42" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="F42" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G42" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H42" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I42" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K42" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="L42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M42" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="N42" s="2" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="2" t="inlineStr">
+        <is>
+          <t>the potcast egypt</t>
+        </is>
+      </c>
+      <c r="B43" s="2" t="inlineStr">
+        <is>
+          <t>https://goocast.net/</t>
+        </is>
+      </c>
+      <c r="C43" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D43" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E43" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="F43" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G43" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H43" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I43" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J43" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K43" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="L43" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M43" s="2" t="n">
+        <v>41.5</v>
+      </c>
+      <c r="N43" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="2" t="inlineStr">
+        <is>
+          <t>video production companies in egypt</t>
+        </is>
+      </c>
+      <c r="B44" s="2" t="inlineStr">
+        <is>
+          <t>https://goocast.net/</t>
+        </is>
+      </c>
+      <c r="C44" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D44" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E44" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="F44" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G44" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H44" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I44" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K44" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M44" s="2" t="n">
+        <v>80</v>
+      </c>
+      <c r="N44" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="2" t="inlineStr">
+        <is>
+          <t>videocast studio</t>
+        </is>
+      </c>
+      <c r="B45" s="2" t="inlineStr">
+        <is>
+          <t>https://goocast.net/</t>
+        </is>
+      </c>
+      <c r="C45" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D45" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E45" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="F45" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G45" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H45" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I45" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K45" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M45" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="N45" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="2" t="inlineStr">
+        <is>
+          <t>vodcast studio</t>
+        </is>
+      </c>
+      <c r="B46" s="2" t="inlineStr">
+        <is>
+          <t>https://goocast.net/</t>
+        </is>
+      </c>
+      <c r="C46" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D46" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E46" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="F46" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G46" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H46" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I46" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K46" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M46" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="N46" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="2" t="inlineStr">
+        <is>
+          <t>استديو بودكاست</t>
+        </is>
+      </c>
+      <c r="B47" s="2" t="inlineStr">
+        <is>
+          <t>https://goocast.net/</t>
+        </is>
+      </c>
+      <c r="C47" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D47" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E47" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="F47" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G47" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H47" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I47" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K47" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="L47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M47" s="2" t="n">
+        <v>74.5</v>
+      </c>
+      <c r="N47" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="inlineStr">
+        <is>
+          <t>استديو تصوير بودكاست</t>
+        </is>
+      </c>
+      <c r="B48" s="2" t="inlineStr">
+        <is>
+          <t>https://goocast.net/</t>
+        </is>
+      </c>
+      <c r="C48" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D48" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E48" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="F48" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G48" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H48" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I48" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K48" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M48" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="N48" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="2" t="inlineStr">
+        <is>
+          <t>استوديو بودكاست</t>
+        </is>
+      </c>
+      <c r="B49" s="2" t="inlineStr">
+        <is>
+          <t>https://goocast.net/</t>
+        </is>
+      </c>
+      <c r="C49" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D49" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E49" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="F49" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G49" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H49" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I49" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J49" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K49" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="L49" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M49" s="2" t="n">
+        <v>40.5</v>
+      </c>
+      <c r="N49" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="2" t="inlineStr">
+        <is>
+          <t>ستوديو بودكاست</t>
+        </is>
+      </c>
+      <c r="B50" s="2" t="inlineStr">
+        <is>
+          <t>https://goocast.net/</t>
+        </is>
+      </c>
+      <c r="C50" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D50" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E50" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="F50" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G50" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H50" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I50" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J50" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K50" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L50" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M50" s="2" t="n">
+        <v>57</v>
+      </c>
+      <c r="N50" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="2" t="inlineStr">
+        <is>
+          <t>gocast</t>
+        </is>
+      </c>
+      <c r="B51" s="2" t="inlineStr">
+        <is>
+          <t>https://goocast.net/contact-us/</t>
+        </is>
+      </c>
+      <c r="C51" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D51" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E51" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="F51" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G51" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H51" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I51" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K51" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="L51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M51" s="2" t="n">
+        <v>62.08</v>
+      </c>
+      <c r="N51" s="2" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="2" t="inlineStr">
+        <is>
+          <t>goocast</t>
+        </is>
+      </c>
+      <c r="B52" s="2" t="inlineStr">
+        <is>
+          <t>https://goocast.net/contact-us/</t>
+        </is>
+      </c>
+      <c r="C52" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D52" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E52" s="4" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="F52" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G52" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H52" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I52" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K52" s="2" t="n">
+        <v>164</v>
+      </c>
+      <c r="L52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M52" s="2" t="n">
+        <v>1.62</v>
+      </c>
+      <c r="N52" s="2" t="n">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -2627,7 +3743,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2636,8 +3752,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="60" customWidth="1" min="1" max="1"/>
-    <col width="30" customWidth="1" min="2" max="2"/>
+    <col width="33" customWidth="1" min="1" max="1"/>
+    <col width="14" customWidth="1" min="2" max="2"/>
     <col width="80" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
@@ -2661,85 +3777,34 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>https://dottopia.com/</t>
+          <t>https://goocast.net/</t>
         </is>
       </c>
       <c r="B2" s="5" t="inlineStr">
         <is>
-          <t>dottopia</t>
+          <t>goocast</t>
         </is>
       </c>
       <c r="C2" s="6" t="inlineStr">
         <is>
-          <t>dotopia; performance marketing agency; advertising agencies; advertising agency cairo; advertising agency egypt; arabic digital marketing agency</t>
+          <t>podcast studio cairo; podcast studio; podcast studios; book podcast studio; podcast locations near me; podcast production studio</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>https://dottopia.com/ar/%D8%A7%D9%81%D8%B6%D9%84-%D8%A7%D8%AF%D8%A7%D9%87-%D9%84%D9%81%D8%AD%D8%B5-%D8%B3%D9%8A%D9%88-%D9%85%D9%88%D9%82%D8%B9%D9%83/</t>
+          <t>https://goocast.net/contact-us/</t>
         </is>
       </c>
       <c r="B3" s="5" t="inlineStr">
         <is>
-          <t>فحص موقعي</t>
+          <t>gocast</t>
         </is>
       </c>
       <c r="C3" s="6" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>https://dottopia.com/ar/%D9%85%D8%B9%D8%A7%D9%8A%D9%8A%D8%B1-%D9%82%D9%8A%D8%A7%D8%B3-%D8%A7%D9%84%D8%A3%D8%AF%D8%A7%D8%A1-%D8%A7%D9%84%D8%AA%D8%B3%D9%88%D9%8A%D9%82%D9%8A/</t>
-        </is>
-      </c>
-      <c r="B4" s="5" t="inlineStr">
-        <is>
-          <t>مؤشرات قياس الأداء التسويقي pdf</t>
-        </is>
-      </c>
-      <c r="C4" s="6" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>https://dottopia.com/types-of-digital-communication-channels/</t>
-        </is>
-      </c>
-      <c r="B5" s="5" t="inlineStr">
-        <is>
-          <t>canales digitales de comunicación</t>
-        </is>
-      </c>
-      <c r="C5" s="6" t="inlineStr">
-        <is>
-          <t>digital communication channels; 7 channels of communication; digital communications; type of communication channel; types of channel in communication; types of digital communication</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>https://dottopia.com/what-is-digital-communication-strategy/</t>
-        </is>
-      </c>
-      <c r="B6" s="5" t="inlineStr">
-        <is>
-          <t>communication strategies that encourage digital connections</t>
-        </is>
-      </c>
-      <c r="C6" s="6" t="inlineStr">
-        <is>
-          <t>describe communication strategies that encourage digital connections. include the following: how does each strategy encourage digital connections? does each strategy work all the time? why or why not?; digital communication strategy; digital marketing communication plan; how does each strategy encourage digital connections?; what is digital communication strategy</t>
+          <t>goocast</t>
         </is>
       </c>
     </row>

</xml_diff>